<commit_message>
dashboard add macro prediction
</commit_message>
<xml_diff>
--- a/PPI-models-public-master/PPI预测模型数据.xlsx
+++ b/PPI-models-public-master/PPI预测模型数据.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\tpy\宏观\PPI\PPI-models-public-master\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\tpy\Data_Tools\PPI-models-public-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDC65670-FC1A-4ADE-8614-ACA3C28A9AEA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F4AB854-6C91-4F15-B979-B99C9DAE2C3E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="15720" activeTab="11" xr2:uid="{A0CF3F64-4DB4-DA47-9097-C5F948AEDDA7}"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28800" windowHeight="15720" firstSheet="8" activeTab="9" xr2:uid="{A0CF3F64-4DB4-DA47-9097-C5F948AEDDA7}"/>
   </bookViews>
   <sheets>
     <sheet name="煤炭" sheetId="11" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="103">
   <si>
     <t>date</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -243,10 +243,6 @@
   </si>
   <si>
     <t>Myspic综合钢价指数:环比:滞后一期</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>11月</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -1080,8 +1076,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C17D365C-C6E1-0E49-BC4B-EF8E890B7E92}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView zoomScale="75" zoomScaleNormal="44" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -1119,7 +1115,7 @@
         <v>9</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -3707,8 +3703,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{22C0F00A-F973-F144-874B-7FF3F4991FAE}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView topLeftCell="A64" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:D79"/>
+    <sheetView tabSelected="1" zoomScale="71" zoomScaleNormal="71" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -3723,13 +3719,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
         <v>30</v>
       </c>
-      <c r="C1" t="s">
-        <v>31</v>
-      </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -5068,9 +5064,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F6D0D5-EC81-4733-8BC4-20110F19CF5E}">
   <dimension ref="A1:P191"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
+    <sheetView topLeftCell="I1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
@@ -5100,96 +5094,96 @@
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B2" t="s">
         <v>50</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>51</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>52</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>53</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>54</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>55</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>56</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>57</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>58</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>59</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>60</v>
       </c>
-      <c r="L2" t="s">
-        <v>61</v>
-      </c>
       <c r="N2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="O2" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" t="s">
         <v>64</v>
-      </c>
-      <c r="P2" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
+        <v>61</v>
+      </c>
+      <c r="O3" t="s">
         <v>62</v>
       </c>
-      <c r="O3" t="s">
-        <v>63</v>
-      </c>
       <c r="P3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.4">
@@ -10305,12 +10299,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D3F1718D-EEF0-42D9-B027-4AAB2EE311B7}">
   <dimension ref="A1:L81"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
+    <col min="1" max="1" width="9.46875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="22.41015625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.46875" bestFit="1" customWidth="1"/>
   </cols>
@@ -10320,37 +10313,37 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C1" t="s">
+        <v>102</v>
+      </c>
+      <c r="D1" t="s">
         <v>93</v>
       </c>
-      <c r="C1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>94</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>95</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>96</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>97</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>98</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>99</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>100</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>101</v>
-      </c>
-      <c r="L1" t="s">
-        <v>102</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.4">
@@ -14294,13 +14287,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="C1" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="C1" s="15" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -16658,7 +16651,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.4">
@@ -18013,10 +18006,10 @@
   <dimension ref="A1:AD86"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B80" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="C91" sqref="C91"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -18063,180 +18056,180 @@
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" t="s">
         <v>69</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>70</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>71</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>72</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>73</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>74</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>75</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>76</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>77</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>78</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>79</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>80</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>81</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>82</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>84</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>85</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>86</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>87</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>88</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>89</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>90</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>91</v>
       </c>
-      <c r="Y2" t="s">
-        <v>92</v>
-      </c>
       <c r="AA2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="AB2" t="s">
+        <v>65</v>
+      </c>
+      <c r="AC2" t="s">
         <v>66</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>67</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.4">
       <c r="A3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B3" t="s">
         <v>62</v>
       </c>
-      <c r="B3" t="s">
-        <v>63</v>
-      </c>
       <c r="C3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="H3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="I3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="K3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="L3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="M3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="N3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="P3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="R3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="S3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="T3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="U3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="V3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="X3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Y3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB3" t="s">
         <v>62</v>
       </c>
-      <c r="AB3" t="s">
-        <v>63</v>
-      </c>
       <c r="AC3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AD3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.4">
@@ -25548,7 +25541,7 @@
         <v>4.0656764685406799</v>
       </c>
       <c r="H86" s="2">
-        <v>0</v>
+        <v>-2.1355799373040663</v>
       </c>
       <c r="I86" s="2">
         <v>0.31714124284158984</v>
@@ -25587,7 +25580,7 @@
         <v>2.304271204474273</v>
       </c>
       <c r="U86" s="2">
-        <v>0</v>
+        <v>2.2418229158642333</v>
       </c>
       <c r="V86" s="2">
         <v>7.5510599460029137</v>
@@ -25613,8 +25606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{551966E9-E27C-694C-97C0-C57F1C92EB9E}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="75" zoomScaleNormal="57" workbookViewId="0">
-      <selection activeCell="F78" sqref="A76:F79"/>
+    <sheetView zoomScale="75" zoomScaleNormal="57" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -25636,7 +25629,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>2</v>
@@ -25645,7 +25638,7 @@
         <v>3</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -27608,8 +27601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CE6D78D-0925-7C40-B9C5-BD00278ADE63}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
-      <selection activeCell="F78" sqref="A77:F79"/>
+    <sheetView zoomScale="58" zoomScaleNormal="58" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -27634,13 +27627,13 @@
         <v>1</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E1" s="4" t="s">
         <v>11</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -29603,8 +29596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEBB0DBB-1534-7A43-AA47-B703CD2D6574}">
   <dimension ref="A1:G91"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="48" workbookViewId="0">
-      <selection activeCell="G78" sqref="A77:G79"/>
+    <sheetView topLeftCell="B1" zoomScale="90" zoomScaleNormal="48" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -29637,7 +29630,7 @@
         <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -32008,8 +32001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C3B749-1BB0-D345-A300-910C17F2692B}">
   <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
-      <selection activeCell="A77" sqref="A77:H79"/>
+    <sheetView topLeftCell="F1" zoomScale="61" zoomScaleNormal="61" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -32045,7 +32038,7 @@
         <v>22</v>
       </c>
       <c r="H1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.4">
@@ -34632,8 +34625,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{56EBDAA8-724B-4A4A-B028-47293B9369C8}">
   <dimension ref="A1:G79"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView topLeftCell="E1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -34651,22 +34644,22 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>41</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.4">
@@ -36941,8 +36934,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{598C949D-4E8F-594F-BC55-6E22CD8AFB3B}">
   <dimension ref="A1:F79"/>
   <sheetViews>
-    <sheetView topLeftCell="B52" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView topLeftCell="E1" zoomScale="63" zoomScaleNormal="63" workbookViewId="0">
+      <selection activeCell="E1" sqref="B1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -36961,19 +36954,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>44</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>45</v>
       </c>
       <c r="E1" s="10" t="s">
         <v>23</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.4">
@@ -38935,8 +38928,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0CC5DB2-DE6A-E14B-B78F-AAD4ECE1E032}">
   <dimension ref="A1:D79"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:D79"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
@@ -38959,7 +38952,7 @@
         <v>25</v>
       </c>
       <c r="D1" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
@@ -40296,2854 +40289,2619 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEA673D2-9917-F44C-BACC-ECB9CAA0A794}">
-  <dimension ref="A1:I79"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView zoomScale="47" zoomScaleNormal="47" workbookViewId="0"/>
+    <sheetView topLeftCell="E1" zoomScale="47" zoomScaleNormal="47" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8203125" defaultRowHeight="15" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="2" width="10.8203125" style="4"/>
-    <col min="3" max="3" width="36.1171875" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.87890625" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="34.3515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="33.8203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="39.8203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.8203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="10" max="16384" width="10.8203125" style="4"/>
+    <col min="1" max="1" width="10.8203125" style="4"/>
+    <col min="2" max="2" width="36.1171875" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.87890625" style="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="34.3515625" style="4" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="33.8203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="39.8203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.8203125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="10.8203125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="7" t="s">
         <v>27</v>
-      </c>
-      <c r="F1" s="7" t="s">
-        <v>36</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="H1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.4">
+      <c r="H1" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A2" s="5">
         <v>41699</v>
       </c>
-      <c r="B2" s="4">
-        <v>0</v>
-      </c>
-      <c r="C2" s="8">
+      <c r="B2" s="8">
         <f>所用指标!AD7</f>
         <v>-7.1607229304502029</v>
       </c>
-      <c r="D2" s="8">
+      <c r="C2" s="8">
         <f>所用指标!AD4</f>
         <v>0.55358350236645038</v>
       </c>
-      <c r="E2" s="9">
+      <c r="D2" s="9">
         <f>所用指标!V9</f>
         <v>1.9740598605569204</v>
       </c>
-      <c r="F2" s="9">
+      <c r="E2" s="9">
         <f>所用指标!W9</f>
         <v>-1.587648227817684</v>
       </c>
-      <c r="G2" s="8">
+      <c r="F2" s="8">
         <f>所用指标!X8</f>
         <v>-3.1783000000000001</v>
       </c>
-      <c r="H2" s="8">
+      <c r="G2" s="8">
         <f>所用指标!X6</f>
         <v>0.56569999999999998</v>
       </c>
-      <c r="I2" s="4">
+      <c r="H2" s="4">
         <f>综合!E9</f>
         <v>-0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A3" s="5">
         <v>41730</v>
       </c>
-      <c r="B3" s="4">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
+      <c r="B3" s="8">
         <f>所用指标!AD8</f>
         <v>-7.0003910833007499</v>
       </c>
-      <c r="D3" s="8">
+      <c r="C3" s="8">
         <f>所用指标!AD5</f>
         <v>-6.7241017020382321</v>
       </c>
-      <c r="E3" s="9">
+      <c r="D3" s="9">
         <f>所用指标!V10</f>
         <v>0.18874946831135553</v>
       </c>
-      <c r="F3" s="9">
+      <c r="E3" s="9">
         <f>所用指标!W10</f>
         <v>-1.2240791931897976</v>
       </c>
-      <c r="G3" s="8">
+      <c r="F3" s="8">
         <f>所用指标!X9</f>
         <v>-7.0799000000000003</v>
       </c>
-      <c r="H3" s="8">
+      <c r="G3" s="8">
         <f>所用指标!X7</f>
         <v>-1.0251999999999999</v>
       </c>
-      <c r="I3" s="4">
+      <c r="H3" s="4">
         <f>综合!E10</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A4" s="5">
         <v>41760</v>
       </c>
-      <c r="B4" s="4">
-        <v>0</v>
-      </c>
-      <c r="C4" s="8">
+      <c r="B4" s="8">
         <f>所用指标!AD9</f>
         <v>10.434538828146911</v>
       </c>
-      <c r="D4" s="8">
+      <c r="C4" s="8">
         <f>所用指标!AD6</f>
         <v>-6.9309904633175652</v>
       </c>
-      <c r="E4" s="9">
+      <c r="D4" s="9">
         <f>所用指标!V11</f>
         <v>1.2345769098097481</v>
       </c>
-      <c r="F4" s="9">
+      <c r="E4" s="9">
         <f>所用指标!W11</f>
         <v>1.1767726475244933</v>
       </c>
-      <c r="G4" s="8">
+      <c r="F4" s="8">
         <f>所用指标!X10</f>
         <v>-6.5772000000000004</v>
       </c>
-      <c r="H4" s="8">
+      <c r="G4" s="8">
         <f>所用指标!X8</f>
         <v>-3.1783000000000001</v>
       </c>
-      <c r="I4" s="4">
+      <c r="H4" s="4">
         <f>综合!E11</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A5" s="5">
         <v>41791</v>
       </c>
-      <c r="B5" s="4">
-        <v>0</v>
-      </c>
-      <c r="C5" s="8">
+      <c r="B5" s="8">
         <f>所用指标!AD10</f>
         <v>5.7194354183590645</v>
       </c>
-      <c r="D5" s="8">
+      <c r="C5" s="8">
         <f>所用指标!AD7</f>
         <v>-7.1607229304502029</v>
       </c>
-      <c r="E5" s="9">
+      <c r="D5" s="9">
         <f>所用指标!V12</f>
         <v>-3.5681358451101541</v>
       </c>
-      <c r="F5" s="9">
+      <c r="E5" s="9">
         <f>所用指标!W12</f>
         <v>1.3787853155133867E-2</v>
       </c>
-      <c r="G5" s="8">
+      <c r="F5" s="8">
         <f>所用指标!X11</f>
         <v>5.6364999999999998</v>
       </c>
-      <c r="H5" s="8">
+      <c r="G5" s="8">
         <f>所用指标!X9</f>
         <v>-7.0799000000000003</v>
       </c>
-      <c r="I5" s="4">
+      <c r="H5" s="4">
         <f>综合!E12</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A6" s="5">
         <v>41821</v>
       </c>
-      <c r="B6" s="4">
-        <v>0</v>
-      </c>
-      <c r="C6" s="8">
+      <c r="B6" s="8">
         <f>所用指标!AD11</f>
         <v>0.12006243246487358</v>
       </c>
-      <c r="D6" s="8">
+      <c r="C6" s="8">
         <f>所用指标!AD8</f>
         <v>-7.0003910833007499</v>
       </c>
-      <c r="E6" s="9">
+      <c r="D6" s="9">
         <f>所用指标!V13</f>
         <v>-5.7087940518453344</v>
       </c>
-      <c r="F6" s="9">
+      <c r="E6" s="9">
         <f>所用指标!W13</f>
         <v>-1.7520882739278099</v>
       </c>
-      <c r="G6" s="8">
+      <c r="F6" s="8">
         <f>所用指标!X12</f>
         <v>2.3740999999999999</v>
       </c>
-      <c r="H6" s="8">
+      <c r="G6" s="8">
         <f>所用指标!X10</f>
         <v>-6.5772000000000004</v>
       </c>
-      <c r="I6" s="4">
+      <c r="H6" s="4">
         <f>综合!E13</f>
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A7" s="5">
         <v>41852</v>
       </c>
-      <c r="B7" s="4">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
+      <c r="B7" s="8">
         <f>所用指标!AD12</f>
         <v>7.1879122196906398</v>
       </c>
-      <c r="D7" s="8">
+      <c r="C7" s="8">
         <f>所用指标!AD9</f>
         <v>10.434538828146911</v>
       </c>
-      <c r="E7" s="9">
+      <c r="D7" s="9">
         <f>所用指标!V14</f>
         <v>-5.383673952808965</v>
       </c>
-      <c r="F7" s="9">
+      <c r="E7" s="9">
         <f>所用指标!W14</f>
         <v>-0.63590374685413842</v>
       </c>
-      <c r="G7" s="8">
+      <c r="F7" s="8">
         <f>所用指标!X13</f>
         <v>0.7278</v>
       </c>
-      <c r="H7" s="8">
+      <c r="G7" s="8">
         <f>所用指标!X11</f>
         <v>5.6364999999999998</v>
       </c>
-      <c r="I7" s="4">
+      <c r="H7" s="4">
         <f>综合!E14</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A8" s="5">
         <v>41883</v>
       </c>
-      <c r="B8" s="4">
-        <v>0</v>
-      </c>
-      <c r="C8" s="8">
+      <c r="B8" s="8">
         <f>所用指标!AD13</f>
         <v>2.1211849995524723</v>
       </c>
-      <c r="D8" s="8">
+      <c r="C8" s="8">
         <f>所用指标!AD10</f>
         <v>5.7194354183590645</v>
       </c>
-      <c r="E8" s="9">
+      <c r="D8" s="9">
         <f>所用指标!V15</f>
         <v>-3.1898363952106767</v>
       </c>
-      <c r="F8" s="9">
+      <c r="E8" s="9">
         <f>所用指标!W15</f>
         <v>0.32460781642076331</v>
       </c>
-      <c r="G8" s="8">
+      <c r="F8" s="8">
         <f>所用指标!X14</f>
         <v>5.0648</v>
       </c>
-      <c r="H8" s="8">
+      <c r="G8" s="8">
         <f>所用指标!X12</f>
         <v>2.3740999999999999</v>
       </c>
-      <c r="I8" s="4">
+      <c r="H8" s="4">
         <f>综合!E15</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A9" s="5">
         <v>41913</v>
       </c>
-      <c r="B9" s="4">
-        <v>0</v>
-      </c>
-      <c r="C9" s="8">
+      <c r="B9" s="8">
         <f>所用指标!AD14</f>
         <v>-3.2690622261174362</v>
       </c>
-      <c r="D9" s="8">
+      <c r="C9" s="8">
         <f>所用指标!AD11</f>
         <v>0.12006243246487358</v>
       </c>
-      <c r="E9" s="9">
+      <c r="D9" s="9">
         <f>所用指标!V16</f>
         <v>-1.9480110775427883</v>
       </c>
-      <c r="F9" s="9">
+      <c r="E9" s="9">
         <f>所用指标!W16</f>
         <v>-0.12507673585729906</v>
       </c>
-      <c r="G9" s="8">
+      <c r="F9" s="8">
         <f>所用指标!X15</f>
         <v>2.3222999999999998</v>
       </c>
-      <c r="H9" s="8">
+      <c r="G9" s="8">
         <f>所用指标!X13</f>
         <v>0.7278</v>
       </c>
-      <c r="I9" s="4">
+      <c r="H9" s="4">
         <f>综合!E16</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A10" s="5">
         <v>41944</v>
       </c>
-      <c r="B10" s="4">
-        <v>1</v>
-      </c>
-      <c r="C10" s="8">
+      <c r="B10" s="8">
         <f>所用指标!AD15</f>
         <v>-1.388511370843537</v>
       </c>
-      <c r="D10" s="8">
+      <c r="C10" s="8">
         <f>所用指标!AD12</f>
         <v>7.1879122196906398</v>
       </c>
-      <c r="E10" s="9">
+      <c r="D10" s="9">
         <f>所用指标!V17</f>
         <v>2.4724780948101488</v>
       </c>
-      <c r="F10" s="9">
+      <c r="E10" s="9">
         <f>所用指标!W17</f>
         <v>-1.5643326548230085</v>
       </c>
-      <c r="G10" s="8">
+      <c r="F10" s="8">
         <f>所用指标!X16</f>
         <v>-0.59</v>
       </c>
-      <c r="H10" s="8">
+      <c r="G10" s="8">
         <f>所用指标!X14</f>
         <v>5.0648</v>
       </c>
-      <c r="I10" s="4">
+      <c r="H10" s="4">
         <f>综合!E17</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A11" s="5">
         <v>41974</v>
       </c>
-      <c r="B11" s="4">
-        <v>0</v>
-      </c>
-      <c r="C11" s="8">
+      <c r="B11" s="8">
         <f>所用指标!AD16</f>
         <v>-1.5389916159411876</v>
       </c>
-      <c r="D11" s="8">
+      <c r="C11" s="8">
         <f>所用指标!AD13</f>
         <v>2.1211849995524723</v>
       </c>
-      <c r="E11" s="9">
+      <c r="D11" s="9">
         <f>所用指标!V18</f>
         <v>-2.5810704342964397</v>
       </c>
-      <c r="F11" s="9">
+      <c r="E11" s="9">
         <f>所用指标!W18</f>
         <v>-0.33453864196665295</v>
       </c>
-      <c r="G11" s="8">
+      <c r="F11" s="8">
         <f>所用指标!X17</f>
         <v>-1.2653000000000001</v>
       </c>
-      <c r="H11" s="8">
+      <c r="G11" s="8">
         <f>所用指标!X15</f>
         <v>2.3222999999999998</v>
       </c>
-      <c r="I11" s="4">
+      <c r="H11" s="4">
         <f>综合!E18</f>
         <v>-0.4</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A12" s="5">
         <v>42005</v>
       </c>
-      <c r="B12" s="4">
-        <v>0</v>
-      </c>
-      <c r="C12" s="8">
+      <c r="B12" s="8">
         <f>所用指标!AD17</f>
         <v>-3.6416656946226644</v>
       </c>
-      <c r="D12" s="8">
+      <c r="C12" s="8">
         <f>所用指标!AD14</f>
         <v>-3.2690622261174362</v>
       </c>
-      <c r="E12" s="9">
+      <c r="D12" s="9">
         <f>所用指标!V19</f>
         <v>0.99866433781978792</v>
       </c>
-      <c r="F12" s="9">
+      <c r="E12" s="9">
         <f>所用指标!W19</f>
         <v>-1.2935526985353163</v>
       </c>
-      <c r="G12" s="8">
+      <c r="F12" s="8">
         <f>所用指标!X18</f>
         <v>-0.54220000000000002</v>
       </c>
-      <c r="H12" s="8">
+      <c r="G12" s="8">
         <f>所用指标!X16</f>
         <v>-0.59</v>
       </c>
-      <c r="I12" s="4">
+      <c r="H12" s="4">
         <f>综合!E19</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A13" s="5">
         <v>42036</v>
       </c>
-      <c r="B13" s="4">
-        <v>0</v>
-      </c>
-      <c r="C13" s="8">
+      <c r="B13" s="8">
         <f>所用指标!AD18</f>
         <v>-3.5686616308347796</v>
       </c>
-      <c r="D13" s="8">
+      <c r="C13" s="8">
         <f>所用指标!AD15</f>
         <v>-1.388511370843537</v>
       </c>
-      <c r="E13" s="9">
+      <c r="D13" s="9">
         <f>所用指标!V20</f>
         <v>-2.8990351404951431</v>
       </c>
-      <c r="F13" s="9">
+      <c r="E13" s="9">
         <f>所用指标!W20</f>
         <v>-0.86808272836803591</v>
       </c>
-      <c r="G13" s="8">
+      <c r="F13" s="8">
         <f>所用指标!X19</f>
         <v>-1.4406000000000001</v>
       </c>
-      <c r="H13" s="8">
+      <c r="G13" s="8">
         <f>所用指标!X17</f>
         <v>-1.2653000000000001</v>
       </c>
-      <c r="I13" s="4">
+      <c r="H13" s="4">
         <f>综合!E20</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A14" s="5">
         <v>42064</v>
       </c>
-      <c r="B14" s="4">
-        <v>0</v>
-      </c>
-      <c r="C14" s="8">
+      <c r="B14" s="8">
         <f>所用指标!AD19</f>
         <v>0.15064022093900231</v>
       </c>
-      <c r="D14" s="8">
+      <c r="C14" s="8">
         <f>所用指标!AD16</f>
         <v>-1.5389916159411876</v>
       </c>
-      <c r="E14" s="9">
+      <c r="D14" s="9">
         <f>所用指标!V21</f>
         <v>1.1336515513126422</v>
       </c>
-      <c r="F14" s="9">
+      <c r="E14" s="9">
         <f>所用指标!W21</f>
         <v>-0.18373391000731099</v>
       </c>
-      <c r="G14" s="8">
+      <c r="F14" s="8">
         <f>所用指标!X20</f>
         <v>0.755</v>
       </c>
-      <c r="H14" s="8">
+      <c r="G14" s="8">
         <f>所用指标!X18</f>
         <v>-0.54220000000000002</v>
       </c>
-      <c r="I14" s="4">
+      <c r="H14" s="4">
         <f>综合!E21</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A15" s="5">
         <v>42095</v>
       </c>
-      <c r="B15" s="4">
-        <v>0</v>
-      </c>
-      <c r="C15" s="8">
+      <c r="B15" s="8">
         <f>所用指标!AD20</f>
         <v>2.093256455251935</v>
       </c>
-      <c r="D15" s="8">
+      <c r="C15" s="8">
         <f>所用指标!AD17</f>
         <v>-3.6416656946226644</v>
       </c>
-      <c r="E15" s="9">
+      <c r="D15" s="9">
         <f>所用指标!V22</f>
         <v>0.99354922363772413</v>
       </c>
-      <c r="F15" s="9">
+      <c r="E15" s="9">
         <f>所用指标!W22</f>
         <v>-2.6274374210187523</v>
       </c>
-      <c r="G15" s="8">
+      <c r="F15" s="8">
         <f>所用指标!X21</f>
         <v>-3.8330000000000002</v>
       </c>
-      <c r="H15" s="8">
+      <c r="G15" s="8">
         <f>所用指标!X19</f>
         <v>-1.4406000000000001</v>
       </c>
-      <c r="I15" s="4">
+      <c r="H15" s="4">
         <f>综合!E22</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A16" s="5">
         <v>42125</v>
       </c>
-      <c r="B16" s="4">
-        <v>0</v>
-      </c>
-      <c r="C16" s="8">
+      <c r="B16" s="8">
         <f>所用指标!AD21</f>
         <v>4.8692449355432599</v>
       </c>
-      <c r="D16" s="8">
+      <c r="C16" s="8">
         <f>所用指标!AD18</f>
         <v>-3.5686616308347796</v>
       </c>
-      <c r="E16" s="9">
+      <c r="D16" s="9">
         <f>所用指标!V23</f>
         <v>1.8572964645086731</v>
       </c>
-      <c r="F16" s="9">
+      <c r="E16" s="9">
         <f>所用指标!W23</f>
         <v>-3.7251876563803243</v>
       </c>
-      <c r="G16" s="8">
+      <c r="F16" s="8">
         <f>所用指标!X22</f>
         <v>-0.77869999999999995</v>
       </c>
-      <c r="H16" s="8">
+      <c r="G16" s="8">
         <f>所用指标!X20</f>
         <v>0.755</v>
       </c>
-      <c r="I16" s="4">
+      <c r="H16" s="4">
         <f>综合!E23</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A17" s="5">
         <v>42156</v>
       </c>
-      <c r="B17" s="4">
-        <v>0</v>
-      </c>
-      <c r="C17" s="8">
+      <c r="B17" s="8">
         <f>所用指标!AD22</f>
         <v>5.7647279198276724</v>
       </c>
-      <c r="D17" s="8">
+      <c r="C17" s="8">
         <f>所用指标!AD19</f>
         <v>0.15064022093900231</v>
       </c>
-      <c r="E17" s="9">
+      <c r="D17" s="9">
         <f>所用指标!V24</f>
         <v>0.32724998148681017</v>
       </c>
-      <c r="F17" s="9">
+      <c r="E17" s="9">
         <f>所用指标!W24</f>
         <v>-1.4584154513204828</v>
       </c>
-      <c r="G17" s="8">
+      <c r="F17" s="8">
         <f>所用指标!X23</f>
         <v>2.6896</v>
       </c>
-      <c r="H17" s="8">
+      <c r="G17" s="8">
         <f>所用指标!X21</f>
         <v>-3.8330000000000002</v>
       </c>
-      <c r="I17" s="4">
+      <c r="H17" s="4">
         <f>综合!E24</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A18" s="5">
         <v>42186</v>
       </c>
-      <c r="B18" s="4">
-        <v>0</v>
-      </c>
-      <c r="C18" s="8">
+      <c r="B18" s="8">
         <f>所用指标!AD23</f>
         <v>11.330529112242637</v>
       </c>
-      <c r="D18" s="8">
+      <c r="C18" s="8">
         <f>所用指标!AD20</f>
         <v>2.093256455251935</v>
       </c>
-      <c r="E18" s="9">
+      <c r="D18" s="9">
         <f>所用指标!V25</f>
         <v>-1.537675788024695</v>
       </c>
-      <c r="F18" s="9">
+      <c r="E18" s="9">
         <f>所用指标!W25</f>
         <v>-0.82853957636565001</v>
       </c>
-      <c r="G18" s="8">
+      <c r="F18" s="8">
         <f>所用指标!X24</f>
         <v>4.0034000000000001</v>
       </c>
-      <c r="H18" s="8">
+      <c r="G18" s="8">
         <f>所用指标!X22</f>
         <v>-0.77869999999999995</v>
       </c>
-      <c r="I18" s="4">
+      <c r="H18" s="4">
         <f>综合!E25</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A19" s="5">
         <v>42217</v>
       </c>
-      <c r="B19" s="4">
-        <v>0</v>
-      </c>
-      <c r="C19" s="8">
+      <c r="B19" s="8">
         <f>所用指标!AD24</f>
         <v>7.8289055042952471</v>
       </c>
-      <c r="D19" s="8">
+      <c r="C19" s="8">
         <f>所用指标!AD21</f>
         <v>4.8692449355432599</v>
       </c>
-      <c r="E19" s="9">
+      <c r="D19" s="9">
         <f>所用指标!V26</f>
         <v>-3.6682366777898823</v>
       </c>
-      <c r="F19" s="9">
+      <c r="E19" s="9">
         <f>所用指标!W26</f>
         <v>-0.40145328968667071</v>
       </c>
-      <c r="G19" s="8">
+      <c r="F19" s="8">
         <f>所用指标!X25</f>
         <v>9.8598999999999997</v>
       </c>
-      <c r="H19" s="8">
+      <c r="G19" s="8">
         <f>所用指标!X23</f>
         <v>2.6896</v>
       </c>
-      <c r="I19" s="4">
+      <c r="H19" s="4">
         <f>综合!E26</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A20" s="5">
         <v>42248</v>
       </c>
-      <c r="B20" s="4">
-        <v>0</v>
-      </c>
-      <c r="C20" s="8">
+      <c r="B20" s="8">
         <f>所用指标!AD25</f>
         <v>0.3596127247579517</v>
       </c>
-      <c r="D20" s="8">
+      <c r="C20" s="8">
         <f>所用指标!AD22</f>
         <v>5.7647279198276724</v>
       </c>
-      <c r="E20" s="9">
+      <c r="D20" s="9">
         <f>所用指标!V27</f>
         <v>-2.2321472920840524</v>
       </c>
-      <c r="F20" s="9">
+      <c r="E20" s="9">
         <f>所用指标!W27</f>
         <v>-2.0700321996218629</v>
       </c>
-      <c r="G20" s="8">
+      <c r="F20" s="8">
         <f>所用指标!X26</f>
         <v>7.7026000000000003</v>
       </c>
-      <c r="H20" s="8">
+      <c r="G20" s="8">
         <f>所用指标!X24</f>
         <v>4.0034000000000001</v>
       </c>
-      <c r="I20" s="4">
+      <c r="H20" s="4">
         <f>综合!E27</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A21" s="5">
         <v>42278</v>
       </c>
-      <c r="B21" s="4">
-        <v>0</v>
-      </c>
-      <c r="C21" s="8">
+      <c r="B21" s="8">
         <f>所用指标!AD26</f>
         <v>-5.1176038221242059</v>
       </c>
-      <c r="D21" s="8">
+      <c r="C21" s="8">
         <f>所用指标!AD23</f>
         <v>11.330529112242637</v>
       </c>
-      <c r="E21" s="9">
+      <c r="D21" s="9">
         <f>所用指标!V28</f>
         <v>1.4299775425222538</v>
       </c>
-      <c r="F21" s="9">
+      <c r="E21" s="9">
         <f>所用指标!W28</f>
         <v>-0.39753869354175464</v>
       </c>
-      <c r="G21" s="8">
+      <c r="F21" s="8">
         <f>所用指标!X27</f>
         <v>0.39450000000000002</v>
       </c>
-      <c r="H21" s="8">
+      <c r="G21" s="8">
         <f>所用指标!X25</f>
         <v>9.8598999999999997</v>
       </c>
-      <c r="I21" s="4">
+      <c r="H21" s="4">
         <f>综合!E28</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A22" s="5">
         <v>42309</v>
       </c>
-      <c r="B22" s="4">
-        <v>1</v>
-      </c>
-      <c r="C22" s="8">
+      <c r="B22" s="8">
         <f>所用指标!AD27</f>
         <v>-6.100513217778647</v>
       </c>
-      <c r="D22" s="8">
+      <c r="C22" s="8">
         <f>所用指标!AD24</f>
         <v>7.8289055042952471</v>
       </c>
-      <c r="E22" s="9">
+      <c r="D22" s="9">
         <f>所用指标!V29</f>
         <v>-1.2509514479195794</v>
       </c>
-      <c r="F22" s="9">
+      <c r="E22" s="9">
         <f>所用指标!W29</f>
         <v>-0.88037391389570452</v>
       </c>
-      <c r="G22" s="8">
+      <c r="F22" s="8">
         <f>所用指标!X28</f>
         <v>-1.9124000000000001</v>
       </c>
-      <c r="H22" s="8">
+      <c r="G22" s="8">
         <f>所用指标!X26</f>
         <v>7.7026000000000003</v>
       </c>
-      <c r="I22" s="4">
+      <c r="H22" s="4">
         <f>综合!E29</f>
         <v>-0.4</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A23" s="5">
         <v>42339</v>
       </c>
-      <c r="B23" s="4">
-        <v>0</v>
-      </c>
-      <c r="C23" s="8">
+      <c r="B23" s="8">
         <f>所用指标!AD28</f>
         <v>-0.37124883984737123</v>
       </c>
-      <c r="D23" s="8">
+      <c r="C23" s="8">
         <f>所用指标!AD25</f>
         <v>0.3596127247579517</v>
       </c>
-      <c r="E23" s="9">
+      <c r="D23" s="9">
         <f>所用指标!V30</f>
         <v>0.9420632913625715</v>
       </c>
-      <c r="F23" s="9">
+      <c r="E23" s="9">
         <f>所用指标!W30</f>
         <v>-4.2827180984217339E-2</v>
       </c>
-      <c r="G23" s="8">
+      <c r="F23" s="8">
         <f>所用指标!X29</f>
         <v>-2.8428</v>
       </c>
-      <c r="H23" s="8">
+      <c r="G23" s="8">
         <f>所用指标!X27</f>
         <v>0.39450000000000002</v>
       </c>
-      <c r="I23" s="4">
+      <c r="H23" s="4">
         <f>综合!E30</f>
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A24" s="5">
         <v>42370</v>
       </c>
-      <c r="B24" s="4">
-        <v>0</v>
-      </c>
-      <c r="C24" s="8">
+      <c r="B24" s="8">
         <f>所用指标!AD29</f>
         <v>7.0365386605941271</v>
       </c>
-      <c r="D24" s="8">
+      <c r="C24" s="8">
         <f>所用指标!AD26</f>
         <v>-5.1176038221242059</v>
       </c>
-      <c r="E24" s="9">
+      <c r="D24" s="9">
         <f>所用指标!V31</f>
         <v>-1.7697707495373804</v>
       </c>
-      <c r="F24" s="9">
+      <c r="E24" s="9">
         <f>所用指标!W31</f>
         <v>-9.2077848059834988E-2</v>
       </c>
-      <c r="G24" s="8">
+      <c r="F24" s="8">
         <f>所用指标!X30</f>
         <v>-0.46510000000000001</v>
       </c>
-      <c r="H24" s="8">
+      <c r="G24" s="8">
         <f>所用指标!X28</f>
         <v>-1.9124000000000001</v>
       </c>
-      <c r="I24" s="4">
+      <c r="H24" s="4">
         <f>综合!E31</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A25" s="5">
         <v>42401</v>
       </c>
-      <c r="B25" s="4">
-        <v>0</v>
-      </c>
-      <c r="C25" s="8">
+      <c r="B25" s="8">
         <f>所用指标!AD30</f>
         <v>4.0796327814740518</v>
       </c>
-      <c r="D25" s="8">
+      <c r="C25" s="8">
         <f>所用指标!AD27</f>
         <v>-6.100513217778647</v>
       </c>
-      <c r="E25" s="9">
+      <c r="D25" s="9">
         <f>所用指标!V32</f>
         <v>-0.27438587696053673</v>
       </c>
-      <c r="F25" s="9">
+      <c r="E25" s="9">
         <f>所用指标!W32</f>
         <v>0.87148546866988585</v>
       </c>
-      <c r="G25" s="8">
+      <c r="F25" s="8">
         <f>所用指标!X31</f>
         <v>2.5</v>
       </c>
-      <c r="H25" s="8">
+      <c r="G25" s="8">
         <f>所用指标!X29</f>
         <v>-2.8428</v>
       </c>
-      <c r="I25" s="4">
+      <c r="H25" s="4">
         <f>综合!E32</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A26" s="5">
         <v>42430</v>
       </c>
-      <c r="B26" s="4">
-        <v>0</v>
-      </c>
-      <c r="C26" s="8">
+      <c r="B26" s="8">
         <f>所用指标!AD31</f>
         <v>0.50483151635283274</v>
       </c>
-      <c r="D26" s="8">
+      <c r="C26" s="8">
         <f>所用指标!AD28</f>
         <v>-0.37124883984737123</v>
       </c>
-      <c r="E26" s="9">
+      <c r="D26" s="9">
         <f>所用指标!V33</f>
         <v>3.3463205110566552</v>
       </c>
-      <c r="F26" s="9">
+      <c r="E26" s="9">
         <f>所用指标!W33</f>
         <v>-1.3149477574809776</v>
       </c>
-      <c r="G26" s="8">
+      <c r="F26" s="8">
         <f>所用指标!X32</f>
         <v>6.3</v>
       </c>
-      <c r="H26" s="8">
+      <c r="G26" s="8">
         <f>所用指标!X30</f>
         <v>-0.46510000000000001</v>
       </c>
-      <c r="I26" s="4">
+      <c r="H26" s="4">
         <f>综合!E33</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A27" s="5">
         <v>42461</v>
       </c>
-      <c r="B27" s="4">
-        <v>0</v>
-      </c>
-      <c r="C27" s="8">
+      <c r="B27" s="8">
         <f>所用指标!AD32</f>
         <v>7.2386058981233292</v>
       </c>
-      <c r="D27" s="8">
+      <c r="C27" s="8">
         <f>所用指标!AD29</f>
         <v>7.0365386605941271</v>
       </c>
-      <c r="E27" s="9">
+      <c r="D27" s="9">
         <f>所用指标!V34</f>
         <v>5.1463812559481514</v>
       </c>
-      <c r="F27" s="9">
+      <c r="E27" s="9">
         <f>所用指标!W34</f>
         <v>-0.85350043215212112</v>
       </c>
-      <c r="G27" s="8">
+      <c r="F27" s="8">
         <f>所用指标!X33</f>
         <v>-1.3</v>
       </c>
-      <c r="H27" s="8">
+      <c r="G27" s="8">
         <f>所用指标!X31</f>
         <v>2.5</v>
       </c>
-      <c r="I27" s="4">
+      <c r="H27" s="4">
         <f>综合!E34</f>
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A28" s="5">
         <v>42491</v>
       </c>
-      <c r="B28" s="4">
-        <v>0</v>
-      </c>
-      <c r="C28" s="8">
+      <c r="B28" s="8">
         <f>所用指标!AD33</f>
         <v>3.137931034482766</v>
       </c>
-      <c r="D28" s="8">
+      <c r="C28" s="8">
         <f>所用指标!AD30</f>
         <v>4.0796327814740518</v>
       </c>
-      <c r="E28" s="9">
+      <c r="D28" s="9">
         <f>所用指标!V35</f>
         <v>-2.2422847701664139E-2</v>
       </c>
-      <c r="F28" s="9">
+      <c r="E28" s="9">
         <f>所用指标!W35</f>
         <v>-1.3164380931625308</v>
       </c>
-      <c r="G28" s="8">
+      <c r="F28" s="8">
         <f>所用指标!X34</f>
         <v>3.2</v>
       </c>
-      <c r="H28" s="8">
+      <c r="G28" s="8">
         <f>所用指标!X32</f>
         <v>6.3</v>
       </c>
-      <c r="I28" s="4">
+      <c r="H28" s="4">
         <f>综合!E35</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A29" s="5">
         <v>42522</v>
       </c>
-      <c r="B29" s="4">
-        <v>0</v>
-      </c>
-      <c r="C29" s="8">
+      <c r="B29" s="8">
         <f>所用指标!AD34</f>
         <v>-1.6466064861250462</v>
       </c>
-      <c r="D29" s="8">
+      <c r="C29" s="8">
         <f>所用指标!AD31</f>
         <v>0.50483151635283274</v>
       </c>
-      <c r="E29" s="9">
+      <c r="D29" s="9">
         <f>所用指标!V36</f>
         <v>2.0881533594598434</v>
       </c>
-      <c r="F29" s="9">
+      <c r="E29" s="9">
         <f>所用指标!W36</f>
         <v>2.3135976443389161E-2</v>
       </c>
-      <c r="G29" s="8">
+      <c r="F29" s="8">
         <f>所用指标!X35</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="H29" s="8">
+      <c r="G29" s="8">
         <f>所用指标!X33</f>
         <v>-1.3</v>
       </c>
-      <c r="I29" s="4">
+      <c r="H29" s="4">
         <f>综合!E36</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A30" s="5">
         <v>42552</v>
       </c>
-      <c r="B30" s="4">
-        <v>0</v>
-      </c>
-      <c r="C30" s="8">
+      <c r="B30" s="8">
         <f>所用指标!AD35</f>
         <v>-5.0293192827398752</v>
       </c>
-      <c r="D30" s="8">
+      <c r="C30" s="8">
         <f>所用指标!AD32</f>
         <v>7.2386058981233292</v>
       </c>
-      <c r="E30" s="9">
+      <c r="D30" s="9">
         <f>所用指标!V37</f>
         <v>3.7174076429438596</v>
       </c>
-      <c r="F30" s="9">
+      <c r="E30" s="9">
         <f>所用指标!W37</f>
         <v>-1.0051307931701392</v>
       </c>
-      <c r="G30" s="8">
+      <c r="F30" s="8">
         <f>所用指标!X36</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H30" s="8">
+      <c r="G30" s="8">
         <f>所用指标!X34</f>
         <v>3.2</v>
       </c>
-      <c r="I30" s="4">
+      <c r="H30" s="4">
         <f>综合!E37</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A31" s="5">
         <v>42583</v>
       </c>
-      <c r="B31" s="4">
-        <v>0</v>
-      </c>
-      <c r="C31" s="8">
+      <c r="B31" s="8">
         <f>所用指标!AD36</f>
         <v>-0.78924761972939406</v>
       </c>
-      <c r="D31" s="8">
+      <c r="C31" s="8">
         <f>所用指标!AD33</f>
         <v>3.137931034482766</v>
       </c>
-      <c r="E31" s="9">
+      <c r="D31" s="9">
         <f>所用指标!V38</f>
         <v>-0.92036256119432114</v>
       </c>
-      <c r="F31" s="9">
+      <c r="E31" s="9">
         <f>所用指标!W38</f>
         <v>-1.5624393929039249</v>
       </c>
-      <c r="G31" s="8">
+      <c r="F31" s="8">
         <f>所用指标!X37</f>
         <v>-2.1</v>
       </c>
-      <c r="H31" s="8">
+      <c r="G31" s="8">
         <f>所用指标!X35</f>
         <v>2.2999999999999998</v>
       </c>
-      <c r="I31" s="4">
+      <c r="H31" s="4">
         <f>综合!E38</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A32" s="5">
         <v>42614</v>
       </c>
-      <c r="B32" s="4">
-        <v>0</v>
-      </c>
-      <c r="C32" s="8">
+      <c r="B32" s="8">
         <f>所用指标!AD37</f>
         <v>-2.6607738793181346</v>
       </c>
-      <c r="D32" s="8">
+      <c r="C32" s="8">
         <f>所用指标!AD34</f>
         <v>-1.6466064861250462</v>
       </c>
-      <c r="E32" s="9">
+      <c r="D32" s="9">
         <f>所用指标!V39</f>
         <v>-0.83132431099666171</v>
       </c>
-      <c r="F32" s="9">
+      <c r="E32" s="9">
         <f>所用指标!W39</f>
         <v>-0.91155068694668273</v>
       </c>
-      <c r="G32" s="8">
+      <c r="F32" s="8">
         <f>所用指标!X38</f>
         <v>-1.2</v>
       </c>
-      <c r="H32" s="8">
+      <c r="G32" s="8">
         <f>所用指标!X36</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I32" s="4">
+      <c r="H32" s="4">
         <f>综合!E39</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A33" s="5">
         <v>42644</v>
       </c>
-      <c r="B33" s="4">
-        <v>0</v>
-      </c>
-      <c r="C33" s="8">
+      <c r="B33" s="8">
         <f>所用指标!AD38</f>
         <v>-6.7210279219174556</v>
       </c>
-      <c r="D33" s="8">
+      <c r="C33" s="8">
         <f>所用指标!AD35</f>
         <v>-5.0293192827398752</v>
       </c>
-      <c r="E33" s="9">
+      <c r="D33" s="9">
         <f>所用指标!V40</f>
         <v>6.7684340947358423</v>
       </c>
-      <c r="F33" s="9">
+      <c r="E33" s="9">
         <f>所用指标!W40</f>
         <v>-0.83968495934959586</v>
       </c>
-      <c r="G33" s="8">
+      <c r="F33" s="8">
         <f>所用指标!X39</f>
         <v>-0.1</v>
       </c>
-      <c r="H33" s="8">
+      <c r="G33" s="8">
         <f>所用指标!X37</f>
         <v>-2.1</v>
       </c>
-      <c r="I33" s="4">
+      <c r="H33" s="4">
         <f>综合!E40</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A34" s="5">
         <v>42675</v>
       </c>
-      <c r="B34" s="4">
-        <v>1</v>
-      </c>
-      <c r="C34" s="8">
+      <c r="B34" s="8">
         <f>所用指标!AD39</f>
         <v>0.57947019867550242</v>
       </c>
-      <c r="D34" s="8">
+      <c r="C34" s="8">
         <f>所用指标!AD36</f>
         <v>-0.78924761972939406</v>
       </c>
-      <c r="E34" s="9">
+      <c r="D34" s="9">
         <f>所用指标!V41</f>
         <v>4.4017501504669543</v>
       </c>
-      <c r="F34" s="9">
+      <c r="E34" s="9">
         <f>所用指标!W41</f>
         <v>0.56553958602409971</v>
       </c>
-      <c r="G34" s="8">
+      <c r="F34" s="8">
         <f>所用指标!X40</f>
         <v>-2.8</v>
       </c>
-      <c r="H34" s="8">
+      <c r="G34" s="8">
         <f>所用指标!X38</f>
         <v>-1.2</v>
       </c>
-      <c r="I34" s="4">
+      <c r="H34" s="4">
         <f>综合!E41</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A35" s="5">
         <v>42705</v>
       </c>
-      <c r="B35" s="4">
-        <v>0</v>
-      </c>
-      <c r="C35" s="8">
+      <c r="B35" s="8">
         <f>所用指标!AD40</f>
         <v>-0.27851851851853349</v>
       </c>
-      <c r="D35" s="8">
+      <c r="C35" s="8">
         <f>所用指标!AD37</f>
         <v>-2.6607738793181346</v>
       </c>
-      <c r="E35" s="9">
+      <c r="D35" s="9">
         <f>所用指标!V42</f>
         <v>6.8401756681478521</v>
       </c>
-      <c r="F35" s="9">
+      <c r="E35" s="9">
         <f>所用指标!W42</f>
         <v>1.7572567616863655</v>
       </c>
-      <c r="G35" s="8">
+      <c r="F35" s="8">
         <f>所用指标!X41</f>
         <v>-1.9</v>
       </c>
-      <c r="H35" s="8">
+      <c r="G35" s="8">
         <f>所用指标!X39</f>
         <v>-0.1</v>
       </c>
-      <c r="I35" s="4">
+      <c r="H35" s="4">
         <f>综合!E42</f>
         <v>0.9</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A36" s="5">
         <v>42736</v>
       </c>
-      <c r="B36" s="4">
-        <v>0</v>
-      </c>
-      <c r="C36" s="8">
+      <c r="B36" s="8">
         <f>所用指标!AD41</f>
         <v>4.3895095475794399</v>
       </c>
-      <c r="D36" s="8">
+      <c r="C36" s="8">
         <f>所用指标!AD38</f>
         <v>-6.7210279219174556</v>
       </c>
-      <c r="E36" s="9">
+      <c r="D36" s="9">
         <f>所用指标!V43</f>
         <v>-4.3989873881593367</v>
       </c>
-      <c r="F36" s="9">
+      <c r="E36" s="9">
         <f>所用指标!W43</f>
         <v>2.1956464431864608</v>
       </c>
-      <c r="G36" s="8">
+      <c r="F36" s="8">
         <f>所用指标!X42</f>
         <v>0.2</v>
       </c>
-      <c r="H36" s="8">
+      <c r="G36" s="8">
         <f>所用指标!X40</f>
         <v>-2.8</v>
       </c>
-      <c r="I36" s="4">
+      <c r="H36" s="4">
         <f>综合!E43</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A37" s="5">
         <v>42767</v>
       </c>
-      <c r="B37" s="4">
-        <v>0</v>
-      </c>
-      <c r="C37" s="8">
+      <c r="B37" s="8">
         <f>所用指标!AD42</f>
         <v>-2.1062618595825366</v>
       </c>
-      <c r="D37" s="8">
+      <c r="C37" s="8">
         <f>所用指标!AD39</f>
         <v>0.57947019867550242</v>
       </c>
-      <c r="E37" s="9">
+      <c r="D37" s="9">
         <f>所用指标!V44</f>
         <v>-1.9935511874496159</v>
       </c>
-      <c r="F37" s="9">
+      <c r="E37" s="9">
         <f>所用指标!W44</f>
         <v>1.6595295291810253</v>
       </c>
-      <c r="G37" s="8">
+      <c r="F37" s="8">
         <f>所用指标!X43</f>
         <v>3.4</v>
       </c>
-      <c r="H37" s="8">
+      <c r="G37" s="8">
         <f>所用指标!X41</f>
         <v>-1.9</v>
       </c>
-      <c r="I37" s="4">
+      <c r="H37" s="4">
         <f>综合!E44</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A38" s="5">
         <v>42795</v>
       </c>
-      <c r="B38" s="4">
-        <v>0</v>
-      </c>
-      <c r="C38" s="8">
+      <c r="B38" s="8">
         <f>所用指标!AD43</f>
         <v>-5.5088195386702736</v>
       </c>
-      <c r="D38" s="8">
+      <c r="C38" s="8">
         <f>所用指标!AD40</f>
         <v>-0.27851851851853349</v>
       </c>
-      <c r="E38" s="9">
+      <c r="D38" s="9">
         <f>所用指标!V45</f>
         <v>-4.7666401211466036</v>
       </c>
-      <c r="F38" s="9">
+      <c r="E38" s="9">
         <f>所用指标!W45</f>
         <v>0.51876708936027249</v>
       </c>
-      <c r="G38" s="8">
+      <c r="F38" s="8">
         <f>所用指标!X44</f>
         <v>-1.6</v>
       </c>
-      <c r="H38" s="8">
+      <c r="G38" s="8">
         <f>所用指标!X42</f>
         <v>0.2</v>
       </c>
-      <c r="I38" s="4">
+      <c r="H38" s="4">
         <f>综合!E45</f>
         <v>-0.4</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A39" s="5">
         <v>42826</v>
       </c>
-      <c r="B39" s="4">
-        <v>0</v>
-      </c>
-      <c r="C39" s="8">
+      <c r="B39" s="8">
         <f>所用指标!AD44</f>
         <v>-1.9652088290801895</v>
       </c>
-      <c r="D39" s="8">
+      <c r="C39" s="8">
         <f>所用指标!AD41</f>
         <v>4.3895095475794399</v>
       </c>
-      <c r="E39" s="9">
+      <c r="D39" s="9">
         <f>所用指标!V46</f>
         <v>-5.6228579846533178</v>
       </c>
-      <c r="F39" s="9">
+      <c r="E39" s="9">
         <f>所用指标!W46</f>
         <v>0.10512391438199931</v>
       </c>
-      <c r="G39" s="8">
+      <c r="F39" s="8">
         <f>所用指标!X45</f>
         <v>-3.5</v>
       </c>
-      <c r="H39" s="8">
+      <c r="G39" s="8">
         <f>所用指标!X43</f>
         <v>3.4</v>
       </c>
-      <c r="I39" s="4">
+      <c r="H39" s="4">
         <f>综合!E46</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A40" s="5">
         <v>42856</v>
       </c>
-      <c r="B40" s="4">
-        <v>0</v>
-      </c>
-      <c r="C40" s="8">
+      <c r="B40" s="8">
         <f>所用指标!AD45</f>
         <v>-3.9443398200460167</v>
       </c>
-      <c r="D40" s="8">
+      <c r="C40" s="8">
         <f>所用指标!AD42</f>
         <v>-2.1062618595825366</v>
       </c>
-      <c r="E40" s="9">
+      <c r="D40" s="9">
         <f>所用指标!V47</f>
         <v>1.4988648962567908</v>
       </c>
-      <c r="F40" s="9">
+      <c r="E40" s="9">
         <f>所用指标!W47</f>
         <v>-0.39263862012480777</v>
       </c>
-      <c r="G40" s="8">
+      <c r="F40" s="8">
         <f>所用指标!X46</f>
         <v>-2</v>
       </c>
-      <c r="H40" s="8">
+      <c r="G40" s="8">
         <f>所用指标!X44</f>
         <v>-1.6</v>
       </c>
-      <c r="I40" s="4">
+      <c r="H40" s="4">
         <f>综合!E47</f>
         <v>-0.4</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A41" s="5">
         <v>42887</v>
       </c>
-      <c r="B41" s="4">
-        <v>0</v>
-      </c>
-      <c r="C41" s="8">
+      <c r="B41" s="8">
         <f>所用指标!AD46</f>
         <v>-7.3913517046073407</v>
       </c>
-      <c r="D41" s="8">
+      <c r="C41" s="8">
         <f>所用指标!AD43</f>
         <v>-5.5088195386702736</v>
       </c>
-      <c r="E41" s="9">
+      <c r="D41" s="9">
         <f>所用指标!V48</f>
         <v>-2.1836737299496645</v>
       </c>
-      <c r="F41" s="9">
+      <c r="E41" s="9">
         <f>所用指标!W48</f>
         <v>-5.2554564003204352E-2</v>
       </c>
-      <c r="G41" s="8">
+      <c r="F41" s="8">
         <f>所用指标!X47</f>
         <v>-2.9</v>
       </c>
-      <c r="H41" s="8">
+      <c r="G41" s="8">
         <f>所用指标!X45</f>
         <v>-3.5</v>
       </c>
-      <c r="I41" s="4">
+      <c r="H41" s="4">
         <f>综合!E48</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A42" s="5">
         <v>42917</v>
       </c>
-      <c r="B42" s="4">
-        <v>0</v>
-      </c>
-      <c r="C42" s="8">
+      <c r="B42" s="8">
         <f>所用指标!AD47</f>
         <v>-1.6748212269476759</v>
       </c>
-      <c r="D42" s="8">
+      <c r="C42" s="8">
         <f>所用指标!AD44</f>
         <v>-1.9652088290801895</v>
       </c>
-      <c r="E42" s="9">
+      <c r="D42" s="9">
         <f>所用指标!V49</f>
         <v>6.5456162741230672</v>
       </c>
-      <c r="F42" s="9">
+      <c r="E42" s="9">
         <f>所用指标!W49</f>
         <v>1.4434328958334852E-2</v>
       </c>
-      <c r="G42" s="8">
+      <c r="F42" s="8">
         <f>所用指标!X48</f>
         <v>-3.4</v>
       </c>
-      <c r="H42" s="8">
+      <c r="G42" s="8">
         <f>所用指标!X46</f>
         <v>-2</v>
       </c>
-      <c r="I42" s="4">
+      <c r="H42" s="4">
         <f>综合!E49</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A43" s="5">
         <v>42948</v>
       </c>
-      <c r="B43" s="4">
-        <v>0</v>
-      </c>
-      <c r="C43" s="8">
+      <c r="B43" s="8">
         <f>所用指标!AD48</f>
         <v>0.83732057416268102</v>
       </c>
-      <c r="D43" s="8">
+      <c r="C43" s="8">
         <f>所用指标!AD45</f>
         <v>-3.9443398200460167</v>
       </c>
-      <c r="E43" s="9">
+      <c r="D43" s="9">
         <f>所用指标!V50</f>
         <v>2.9742116364456894</v>
       </c>
-      <c r="F43" s="9">
+      <c r="E43" s="9">
         <f>所用指标!W50</f>
         <v>-1.7480049213081106E-2</v>
       </c>
-      <c r="G43" s="8">
+      <c r="F43" s="8">
         <f>所用指标!X49</f>
         <v>-0.7</v>
       </c>
-      <c r="H43" s="8">
+      <c r="G43" s="8">
         <f>所用指标!X47</f>
         <v>-2.9</v>
       </c>
-      <c r="I43" s="4">
+      <c r="H43" s="4">
         <f>综合!E50</f>
         <v>0.5</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A44" s="5">
         <v>42979</v>
       </c>
-      <c r="B44" s="4">
-        <v>0</v>
-      </c>
-      <c r="C44" s="8">
+      <c r="B44" s="8">
         <f>所用指标!AD49</f>
         <v>1.2858837485171692</v>
       </c>
-      <c r="D44" s="8">
+      <c r="C44" s="8">
         <f>所用指标!AD46</f>
         <v>-7.3913517046073407</v>
       </c>
-      <c r="E44" s="9">
+      <c r="D44" s="9">
         <f>所用指标!V51</f>
         <v>-0.1449843425339381</v>
       </c>
-      <c r="F44" s="9">
+      <c r="E44" s="9">
         <f>所用指标!W51</f>
         <v>3.4411947196131942</v>
       </c>
-      <c r="G44" s="8">
+      <c r="F44" s="8">
         <f>所用指标!X50</f>
         <v>1.3</v>
       </c>
-      <c r="H44" s="8">
+      <c r="G44" s="8">
         <f>所用指标!X48</f>
         <v>-3.4</v>
       </c>
-      <c r="I44" s="4">
+      <c r="H44" s="4">
         <f>综合!E51</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A45" s="5">
         <v>43009</v>
       </c>
-      <c r="B45" s="4">
-        <v>0</v>
-      </c>
-      <c r="C45" s="8">
+      <c r="B45" s="8">
         <f>所用指标!AD50</f>
         <v>-0.52781161185544434</v>
       </c>
-      <c r="D45" s="8">
+      <c r="C45" s="8">
         <f>所用指标!AD47</f>
         <v>-1.6748212269476759</v>
       </c>
-      <c r="E45" s="9">
+      <c r="D45" s="9">
         <f>所用指标!V52</f>
         <v>-2.2088089677187117</v>
       </c>
-      <c r="F45" s="9">
+      <c r="E45" s="9">
         <f>所用指标!W52</f>
         <v>3.6077215012052521</v>
       </c>
-      <c r="G45" s="8">
+      <c r="F45" s="8">
         <f>所用指标!X51</f>
         <v>1</v>
       </c>
-      <c r="H45" s="8">
+      <c r="G45" s="8">
         <f>所用指标!X49</f>
         <v>-0.7</v>
       </c>
-      <c r="I45" s="4">
+      <c r="H45" s="4">
         <f>综合!E52</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A46" s="5">
         <v>43040</v>
       </c>
-      <c r="B46" s="4">
-        <v>1</v>
-      </c>
-      <c r="C46" s="8">
+      <c r="B46" s="8">
         <f>所用指标!AD51</f>
         <v>-0.87519623233909272</v>
       </c>
-      <c r="D46" s="8">
+      <c r="C46" s="8">
         <f>所用指标!AD48</f>
         <v>0.83732057416268102</v>
       </c>
-      <c r="E46" s="9">
+      <c r="D46" s="9">
         <f>所用指标!V53</f>
         <v>1.7217353359462173</v>
       </c>
-      <c r="F46" s="9">
+      <c r="E46" s="9">
         <f>所用指标!W53</f>
         <v>2.7808268312867535</v>
       </c>
-      <c r="G46" s="8">
+      <c r="F46" s="8">
         <f>所用指标!X52</f>
         <v>-0.1</v>
       </c>
-      <c r="H46" s="8">
+      <c r="G46" s="8">
         <f>所用指标!X50</f>
         <v>1.3</v>
       </c>
-      <c r="I46" s="4">
+      <c r="H46" s="4">
         <f>综合!E53</f>
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A47" s="5">
         <v>43070</v>
       </c>
-      <c r="B47" s="4">
-        <v>0</v>
-      </c>
-      <c r="C47" s="8">
+      <c r="B47" s="8">
         <f>所用指标!AD52</f>
         <v>3.8128043710654591</v>
       </c>
-      <c r="D47" s="8">
+      <c r="C47" s="8">
         <f>所用指标!AD49</f>
         <v>1.2858837485171692</v>
       </c>
-      <c r="E47" s="9">
+      <c r="D47" s="9">
         <f>所用指标!V54</f>
         <v>-3.2614206121072797</v>
       </c>
-      <c r="F47" s="9">
+      <c r="E47" s="9">
         <f>所用指标!W54</f>
         <v>3.2202836729162909</v>
       </c>
-      <c r="G47" s="8">
+      <c r="F47" s="8">
         <f>所用指标!X53</f>
         <v>-0.8</v>
       </c>
-      <c r="H47" s="8">
+      <c r="G47" s="8">
         <f>所用指标!X51</f>
         <v>1</v>
       </c>
-      <c r="I47" s="4">
+      <c r="H47" s="4">
         <f>综合!E54</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A48" s="5">
         <v>43101</v>
       </c>
-      <c r="B48" s="4">
-        <v>0</v>
-      </c>
-      <c r="C48" s="8">
+      <c r="B48" s="8">
         <f>所用指标!AD53</f>
         <v>0.30892448512582771</v>
       </c>
-      <c r="D48" s="8">
+      <c r="C48" s="8">
         <f>所用指标!AD50</f>
         <v>-0.52781161185544434</v>
       </c>
-      <c r="E48" s="9">
+      <c r="D48" s="9">
         <f>所用指标!V55</f>
         <v>-1.4763932978635652</v>
       </c>
-      <c r="F48" s="9">
+      <c r="E48" s="9">
         <f>所用指标!W55</f>
         <v>1.9525801377700214</v>
       </c>
-      <c r="G48" s="8">
+      <c r="F48" s="8">
         <f>所用指标!X54</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H48" s="8">
+      <c r="G48" s="8">
         <f>所用指标!X52</f>
         <v>-0.1</v>
       </c>
-      <c r="I48" s="4">
+      <c r="H48" s="4">
         <f>综合!E55</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A49" s="5">
         <v>43132</v>
       </c>
-      <c r="B49" s="4">
-        <v>0</v>
-      </c>
-      <c r="C49" s="8">
+      <c r="B49" s="8">
         <f>所用指标!AD54</f>
         <v>-2.8173833694536188</v>
       </c>
-      <c r="D49" s="8">
+      <c r="C49" s="8">
         <f>所用指标!AD51</f>
         <v>-0.87519623233909272</v>
       </c>
-      <c r="E49" s="9">
+      <c r="D49" s="9">
         <f>所用指标!V56</f>
         <v>-2.7498836451642972</v>
       </c>
-      <c r="F49" s="9">
+      <c r="E49" s="9">
         <f>所用指标!W56</f>
         <v>2.3786015259367854</v>
       </c>
-      <c r="G49" s="8">
+      <c r="F49" s="8">
         <f>所用指标!X55</f>
         <v>0.7</v>
       </c>
-      <c r="H49" s="8">
+      <c r="G49" s="8">
         <f>所用指标!X53</f>
         <v>-0.8</v>
       </c>
-      <c r="I49" s="4">
+      <c r="H49" s="4">
         <f>综合!E56</f>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A50" s="5">
         <v>43160</v>
       </c>
-      <c r="B50" s="4">
-        <v>0</v>
-      </c>
-      <c r="C50" s="8">
+      <c r="B50" s="8">
         <f>所用指标!AD55</f>
         <v>-8.3755868544601046</v>
       </c>
-      <c r="D50" s="8">
+      <c r="C50" s="8">
         <f>所用指标!AD52</f>
         <v>3.8128043710654591</v>
       </c>
-      <c r="E50" s="9">
+      <c r="D50" s="9">
         <f>所用指标!V57</f>
         <v>1.1435184033048662</v>
       </c>
-      <c r="F50" s="9">
+      <c r="E50" s="9">
         <f>所用指标!W57</f>
         <v>-0.1348333461792417</v>
       </c>
-      <c r="G50" s="8">
+      <c r="F50" s="8">
         <f>所用指标!X56</f>
         <v>2</v>
       </c>
-      <c r="H50" s="8">
+      <c r="G50" s="8">
         <f>所用指标!X54</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I50" s="4">
+      <c r="H50" s="4">
         <f>综合!E57</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A51" s="5">
         <v>43191</v>
       </c>
-      <c r="B51" s="4">
-        <v>0</v>
-      </c>
-      <c r="C51" s="8">
+      <c r="B51" s="8">
         <f>所用指标!AD56</f>
         <v>-10.107945617271296</v>
       </c>
-      <c r="D51" s="8">
+      <c r="C51" s="8">
         <f>所用指标!AD53</f>
         <v>0.30892448512582771</v>
       </c>
-      <c r="E51" s="9">
+      <c r="D51" s="9">
         <f>所用指标!V58</f>
         <v>2.0429858222809072</v>
       </c>
-      <c r="F51" s="9">
+      <c r="E51" s="9">
         <f>所用指标!W58</f>
         <v>-0.19597747919817277</v>
       </c>
-      <c r="G51" s="8">
+      <c r="F51" s="8">
         <f>所用指标!X57</f>
         <v>-8.4</v>
       </c>
-      <c r="H51" s="8">
+      <c r="G51" s="8">
         <f>所用指标!X55</f>
         <v>0.7</v>
       </c>
-      <c r="I51" s="4">
+      <c r="H51" s="4">
         <f>综合!E58</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A52" s="5">
         <v>43221</v>
       </c>
-      <c r="B52" s="4">
-        <v>0</v>
-      </c>
-      <c r="C52" s="8">
+      <c r="B52" s="8">
         <f>所用指标!AD57</f>
         <v>-5.1206536196085839</v>
       </c>
-      <c r="D52" s="8">
+      <c r="C52" s="8">
         <f>所用指标!AD54</f>
         <v>-2.8173833694536188</v>
       </c>
-      <c r="E52" s="9">
+      <c r="D52" s="9">
         <f>所用指标!V59</f>
         <v>2.085626051043632</v>
       </c>
-      <c r="F52" s="9">
+      <c r="E52" s="9">
         <f>所用指标!W59</f>
         <v>-0.37525169320885565</v>
       </c>
-      <c r="G52" s="8">
+      <c r="F52" s="8">
         <f>所用指标!X58</f>
         <v>-6.6</v>
       </c>
-      <c r="H52" s="8">
+      <c r="G52" s="8">
         <f>所用指标!X56</f>
         <v>2</v>
       </c>
-      <c r="I52" s="4">
+      <c r="H52" s="4">
         <f>综合!E59</f>
         <v>0</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A53" s="5">
         <v>43252</v>
       </c>
-      <c r="B53" s="4">
-        <v>0</v>
-      </c>
-      <c r="C53" s="8">
+      <c r="B53" s="8">
         <f>所用指标!AD58</f>
         <v>5.8455992790628075</v>
       </c>
-      <c r="D53" s="8">
+      <c r="C53" s="8">
         <f>所用指标!AD55</f>
         <v>-8.3755868544601046</v>
       </c>
-      <c r="E53" s="9">
+      <c r="D53" s="9">
         <f>所用指标!V60</f>
         <v>-0.2407151276478281</v>
       </c>
-      <c r="F53" s="9">
+      <c r="E53" s="9">
         <f>所用指标!W60</f>
         <v>0.36380339917319038</v>
       </c>
-      <c r="G53" s="8">
+      <c r="F53" s="8">
         <f>所用指标!X59</f>
         <v>-3.6</v>
       </c>
-      <c r="H53" s="8">
+      <c r="G53" s="8">
         <f>所用指标!X57</f>
         <v>-8.4</v>
       </c>
-      <c r="I53" s="4">
+      <c r="H53" s="4">
         <f>综合!E60</f>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A54" s="5">
         <v>43282</v>
       </c>
-      <c r="B54" s="4">
-        <v>0</v>
-      </c>
-      <c r="C54" s="8">
+      <c r="B54" s="8">
         <f>所用指标!AD59</f>
         <v>3.4879100919514183</v>
       </c>
-      <c r="D54" s="8">
+      <c r="C54" s="8">
         <f>所用指标!AD56</f>
         <v>-10.107945617271296</v>
       </c>
-      <c r="E54" s="9">
+      <c r="D54" s="9">
         <f>所用指标!V61</f>
         <v>-1.660113497206972</v>
       </c>
-      <c r="F54" s="9">
+      <c r="E54" s="9">
         <f>所用指标!W61</f>
         <v>0.22501343922720629</v>
       </c>
-      <c r="G54" s="8">
+      <c r="F54" s="8">
         <f>所用指标!X60</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="H54" s="8">
+      <c r="G54" s="8">
         <f>所用指标!X58</f>
         <v>-6.6</v>
       </c>
-      <c r="I54" s="4">
+      <c r="H54" s="4">
         <f>综合!E61</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A55" s="5">
         <v>43313</v>
       </c>
-      <c r="B55" s="4">
-        <v>0</v>
-      </c>
-      <c r="C55" s="8">
+      <c r="B55" s="8">
         <f>所用指标!AD60</f>
         <v>10.165912518853681</v>
       </c>
-      <c r="D55" s="8">
+      <c r="C55" s="8">
         <f>所用指标!AD57</f>
         <v>-5.1206536196085839</v>
       </c>
-      <c r="E55" s="9">
+      <c r="D55" s="9">
         <f>所用指标!V62</f>
         <v>1.4748614080800193</v>
       </c>
-      <c r="F55" s="9">
+      <c r="E55" s="9">
         <f>所用指标!W62</f>
         <v>0.92395952122326097</v>
       </c>
-      <c r="G55" s="8">
+      <c r="F55" s="8">
         <f>所用指标!X61</f>
         <v>2.9</v>
       </c>
-      <c r="H55" s="8">
+      <c r="G55" s="8">
         <f>所用指标!X59</f>
         <v>-3.6</v>
       </c>
-      <c r="I55" s="4">
+      <c r="H55" s="4">
         <f>综合!E62</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A56" s="5">
         <v>43344</v>
       </c>
-      <c r="B56" s="4">
-        <v>0</v>
-      </c>
-      <c r="C56" s="8">
+      <c r="B56" s="8">
         <f>所用指标!AD61</f>
         <v>6.940157323508922</v>
       </c>
-      <c r="D56" s="8">
+      <c r="C56" s="8">
         <f>所用指标!AD58</f>
         <v>5.8455992790628075</v>
       </c>
-      <c r="E56" s="9">
+      <c r="D56" s="9">
         <f>所用指标!V63</f>
         <v>0.76360443898055852</v>
       </c>
-      <c r="F56" s="9">
+      <c r="E56" s="9">
         <f>所用指标!W63</f>
         <v>0.5139660031499016</v>
       </c>
-      <c r="G56" s="8">
+      <c r="F56" s="8">
         <f>所用指标!X62</f>
         <v>6.5</v>
       </c>
-      <c r="H56" s="8">
+      <c r="G56" s="8">
         <f>所用指标!X60</f>
         <v>1.1000000000000001</v>
       </c>
-      <c r="I56" s="4">
+      <c r="H56" s="4">
         <f>综合!E63</f>
         <v>0.6</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A57" s="5">
         <v>43374</v>
       </c>
-      <c r="B57" s="4">
-        <v>0</v>
-      </c>
-      <c r="C57" s="8">
+      <c r="B57" s="8">
         <f>所用指标!AD62</f>
         <v>-1.3151769087523246</v>
       </c>
-      <c r="D57" s="8">
+      <c r="C57" s="8">
         <f>所用指标!AD59</f>
         <v>3.4879100919514183</v>
       </c>
-      <c r="E57" s="9">
+      <c r="D57" s="9">
         <f>所用指标!V64</f>
         <v>-0.15349324944292642</v>
       </c>
-      <c r="F57" s="9">
+      <c r="E57" s="9">
         <f>所用指标!W64</f>
         <v>1.6362986780993349</v>
       </c>
-      <c r="G57" s="8">
+      <c r="F57" s="8">
         <f>所用指标!X63</f>
         <v>3.7</v>
       </c>
-      <c r="H57" s="8">
+      <c r="G57" s="8">
         <f>所用指标!X61</f>
         <v>2.9</v>
       </c>
-      <c r="I57" s="4">
+      <c r="H57" s="4">
         <f>综合!E64</f>
         <v>0</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A58" s="5">
         <v>43405</v>
       </c>
-      <c r="B58" s="4">
-        <v>1</v>
-      </c>
-      <c r="C58" s="8">
+      <c r="B58" s="8">
         <f>所用指标!AD63</f>
         <v>-2.8092935487675441</v>
       </c>
-      <c r="D58" s="8">
+      <c r="C58" s="8">
         <f>所用指标!AD60</f>
         <v>10.165912518853681</v>
       </c>
-      <c r="E58" s="9">
+      <c r="D58" s="9">
         <f>所用指标!V65</f>
         <v>-4.3056591708408698</v>
       </c>
-      <c r="F58" s="9">
+      <c r="E58" s="9">
         <f>所用指标!W65</f>
         <v>4.2183249821044599</v>
       </c>
-      <c r="G58" s="8">
+      <c r="F58" s="8">
         <f>所用指标!X64</f>
         <v>1</v>
       </c>
-      <c r="H58" s="8">
+      <c r="G58" s="8">
         <f>所用指标!X62</f>
         <v>6.5</v>
       </c>
-      <c r="I58" s="4">
+      <c r="H58" s="4">
         <f>综合!E65</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A59" s="5">
         <v>43435</v>
       </c>
-      <c r="B59" s="4">
-        <v>0</v>
-      </c>
-      <c r="C59" s="8">
+      <c r="B59" s="8">
         <f>所用指标!AD64</f>
         <v>0.96107174060771072</v>
       </c>
-      <c r="D59" s="8">
+      <c r="C59" s="8">
         <f>所用指标!AD61</f>
         <v>6.940157323508922</v>
       </c>
-      <c r="E59" s="9">
+      <c r="D59" s="9">
         <f>所用指标!V66</f>
         <v>2.7902694940677097</v>
       </c>
-      <c r="F59" s="9">
+      <c r="E59" s="9">
         <f>所用指标!W66</f>
         <v>3.3379989815052191</v>
       </c>
-      <c r="G59" s="8">
+      <c r="F59" s="8">
         <f>所用指标!X65</f>
         <v>-0.6</v>
       </c>
-      <c r="H59" s="8">
+      <c r="G59" s="8">
         <f>所用指标!X63</f>
         <v>3.7</v>
       </c>
-      <c r="I59" s="4">
+      <c r="H59" s="4">
         <f>综合!E66</f>
         <v>-0.1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A60" s="5">
         <v>43466</v>
       </c>
-      <c r="B60" s="4">
-        <v>0</v>
-      </c>
-      <c r="C60" s="8">
+      <c r="B60" s="8">
         <f>所用指标!AD65</f>
         <v>-4.2187500000000044</v>
       </c>
-      <c r="D60" s="8">
+      <c r="C60" s="8">
         <f>所用指标!AD62</f>
         <v>-1.3151769087523246</v>
       </c>
-      <c r="E60" s="9">
+      <c r="D60" s="9">
         <f>所用指标!V67</f>
         <v>-5.6087266530713276E-2</v>
       </c>
-      <c r="F60" s="9">
+      <c r="E60" s="9">
         <f>所用指标!W67</f>
         <v>3.2325614021094795</v>
       </c>
-      <c r="G60" s="8">
+      <c r="F60" s="8">
         <f>所用指标!X66</f>
         <v>0.7</v>
       </c>
-      <c r="H60" s="8">
+      <c r="G60" s="8">
         <f>所用指标!X64</f>
         <v>1</v>
       </c>
-      <c r="I60" s="4">
+      <c r="H60" s="4">
         <f>综合!E67</f>
         <v>-0.3</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A61" s="5">
         <v>43497</v>
       </c>
-      <c r="B61" s="4">
-        <v>0</v>
-      </c>
-      <c r="C61" s="8">
+      <c r="B61" s="8">
         <f>所用指标!AD66</f>
         <v>-3.8273309072656692</v>
       </c>
-      <c r="D61" s="8">
+      <c r="C61" s="8">
         <f>所用指标!AD63</f>
         <v>-2.8092935487675441</v>
       </c>
-      <c r="E61" s="9">
+      <c r="D61" s="9">
         <f>所用指标!V68</f>
         <v>1.6857765629865629</v>
       </c>
-      <c r="F61" s="9">
+      <c r="E61" s="9">
         <f>所用指标!W68</f>
         <v>1.8129077806888327</v>
       </c>
-      <c r="G61" s="8">
+      <c r="F61" s="8">
         <f>所用指标!X67</f>
         <v>-1</v>
       </c>
-      <c r="H61" s="8">
+      <c r="G61" s="8">
         <f>所用指标!X65</f>
         <v>-0.6</v>
       </c>
-      <c r="I61" s="4">
+      <c r="H61" s="4">
         <f>综合!E68</f>
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A62" s="5">
         <v>43525</v>
       </c>
-      <c r="B62" s="4">
-        <v>0</v>
-      </c>
-      <c r="C62" s="8">
+      <c r="B62" s="8">
         <f>所用指标!AD67</f>
         <v>10.344467640918587</v>
       </c>
-      <c r="D62" s="8">
+      <c r="C62" s="8">
         <f>所用指标!AD64</f>
         <v>0.96107174060771072</v>
       </c>
-      <c r="E62" s="9">
+      <c r="D62" s="9">
         <f>所用指标!V69</f>
         <v>4.7489299330726986</v>
       </c>
-      <c r="F62" s="9">
+      <c r="E62" s="9">
         <f>所用指标!W69</f>
         <v>-4.2420743063373738</v>
       </c>
-      <c r="G62" s="8">
+      <c r="F62" s="8">
         <f>所用指标!X68</f>
         <v>0.3</v>
       </c>
-      <c r="H62" s="8">
+      <c r="G62" s="8">
         <f>所用指标!X66</f>
         <v>0.7</v>
       </c>
-      <c r="I62" s="4">
+      <c r="H62" s="4">
         <f>综合!E69</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A63" s="5">
         <v>43556</v>
       </c>
-      <c r="B63" s="4">
-        <v>0</v>
-      </c>
-      <c r="C63" s="8">
+      <c r="B63" s="8">
         <f>所用指标!AD68</f>
         <v>8.1614795194399736</v>
       </c>
-      <c r="D63" s="8">
+      <c r="C63" s="8">
         <f>所用指标!AD65</f>
         <v>-4.2187500000000044</v>
       </c>
-      <c r="E63" s="9">
+      <c r="D63" s="9">
         <f>所用指标!V70</f>
         <v>-0.11093491591405158</v>
       </c>
-      <c r="F63" s="9">
+      <c r="E63" s="9">
         <f>所用指标!W70</f>
         <v>-2.2750091806995498</v>
       </c>
-      <c r="G63" s="8">
+      <c r="F63" s="8">
         <f>所用指标!X69</f>
         <v>1.2</v>
       </c>
-      <c r="H63" s="8">
+      <c r="G63" s="8">
         <f>所用指标!X67</f>
         <v>-1</v>
       </c>
-      <c r="I63" s="4">
+      <c r="H63" s="4">
         <f>综合!E70</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A64" s="5">
         <v>43586</v>
       </c>
-      <c r="B64" s="4">
-        <v>0</v>
-      </c>
-      <c r="C64" s="8">
+      <c r="B64" s="8">
         <f>所用指标!AD69</f>
         <v>2.6128785394118115</v>
       </c>
-      <c r="D64" s="8">
+      <c r="C64" s="8">
         <f>所用指标!AD66</f>
         <v>-3.8273309072656692</v>
       </c>
-      <c r="E64" s="9">
+      <c r="D64" s="9">
         <f>所用指标!V71</f>
         <v>0.34772092389452336</v>
       </c>
-      <c r="F64" s="9">
+      <c r="E64" s="9">
         <f>所用指标!W71</f>
         <v>0.61322597263058221</v>
       </c>
-      <c r="G64" s="8">
+      <c r="F64" s="8">
         <f>所用指标!X70</f>
         <v>1.6</v>
       </c>
-      <c r="H64" s="8">
+      <c r="G64" s="8">
         <f>所用指标!X68</f>
         <v>0.3</v>
       </c>
-      <c r="I64" s="4">
+      <c r="H64" s="4">
         <f>综合!E71</f>
         <v>0.3</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A65" s="5">
         <v>43617</v>
       </c>
-      <c r="B65" s="4">
-        <v>0</v>
-      </c>
-      <c r="C65" s="8">
+      <c r="B65" s="8">
         <f>所用指标!AD70</f>
         <v>3.4945663754528233</v>
       </c>
-      <c r="D65" s="8">
+      <c r="C65" s="8">
         <f>所用指标!AD67</f>
         <v>10.344467640918587</v>
       </c>
-      <c r="E65" s="9">
+      <c r="D65" s="9">
         <f>所用指标!V72</f>
         <v>-5.301918559079688E-2</v>
       </c>
-      <c r="F65" s="9">
+      <c r="E65" s="9">
         <f>所用指标!W72</f>
         <v>1.7429883738689478</v>
       </c>
-      <c r="G65" s="8">
+      <c r="F65" s="8">
         <f>所用指标!X71</f>
         <v>-0.3</v>
       </c>
-      <c r="H65" s="8">
+      <c r="G65" s="8">
         <f>所用指标!X69</f>
         <v>1.2</v>
       </c>
-      <c r="I65" s="4">
+      <c r="H65" s="4">
         <f>综合!E72</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A66" s="5">
         <v>43647</v>
       </c>
-      <c r="B66" s="4">
-        <v>0</v>
-      </c>
-      <c r="C66" s="8">
+      <c r="B66" s="8">
         <f>所用指标!AD71</f>
         <v>8.8737904056001682</v>
       </c>
-      <c r="D66" s="8">
+      <c r="C66" s="8">
         <f>所用指标!AD68</f>
         <v>8.1614795194399736</v>
       </c>
-      <c r="E66" s="9">
+      <c r="D66" s="9">
         <f>所用指标!V73</f>
         <v>-1.494543793779668</v>
       </c>
-      <c r="F66" s="9">
+      <c r="E66" s="9">
         <f>所用指标!W73</f>
         <v>1.9089015771984519</v>
       </c>
-      <c r="G66" s="8">
+      <c r="F66" s="8">
         <f>所用指标!X72</f>
         <v>3.6</v>
       </c>
-      <c r="H66" s="8">
+      <c r="G66" s="8">
         <f>所用指标!X70</f>
         <v>1.6</v>
       </c>
-      <c r="I66" s="4">
+      <c r="H66" s="4">
         <f>综合!E73</f>
         <v>0.1</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A67" s="5">
         <v>43678</v>
       </c>
-      <c r="B67" s="4">
-        <v>0</v>
-      </c>
-      <c r="C67" s="8">
+      <c r="B67" s="8">
         <f>所用指标!AD72</f>
         <v>18.66868381240543</v>
       </c>
-      <c r="D67" s="8">
+      <c r="C67" s="8">
         <f>所用指标!AD69</f>
         <v>2.6128785394118115</v>
       </c>
-      <c r="E67" s="9">
+      <c r="D67" s="9">
         <f>所用指标!V74</f>
         <v>5.6204534578335075</v>
       </c>
-      <c r="F67" s="9">
+      <c r="E67" s="9">
         <f>所用指标!W74</f>
         <v>2.1770071443146133</v>
       </c>
-      <c r="G67" s="8">
+      <c r="F67" s="8">
         <f>所用指标!X73</f>
         <v>7.8</v>
       </c>
-      <c r="H67" s="8">
+      <c r="G67" s="8">
         <f>所用指标!X71</f>
         <v>-0.3</v>
       </c>
-      <c r="I67" s="4">
+      <c r="H67" s="4">
         <f>综合!E74</f>
         <v>1.4</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A68" s="5">
         <v>43709</v>
       </c>
-      <c r="B68" s="4">
-        <v>0</v>
-      </c>
-      <c r="C68" s="8">
+      <c r="B68" s="8">
         <f>所用指标!AD73</f>
         <v>21.948304436512011</v>
       </c>
-      <c r="D68" s="8">
+      <c r="C68" s="8">
         <f>所用指标!AD70</f>
         <v>3.4945663754528233</v>
       </c>
-      <c r="E68" s="9">
+      <c r="D68" s="9">
         <f>所用指标!V75</f>
         <v>0.64508086883356963</v>
       </c>
-      <c r="F68" s="9">
+      <c r="E68" s="9">
         <f>所用指标!W75</f>
         <v>4.3487091287502722</v>
       </c>
-      <c r="G68" s="8">
+      <c r="F68" s="8">
         <f>所用指标!X74</f>
         <v>23.1</v>
       </c>
-      <c r="H68" s="8">
+      <c r="G68" s="8">
         <f>所用指标!X72</f>
         <v>3.6</v>
       </c>
-      <c r="I68" s="4">
+      <c r="H68" s="4">
         <f>综合!E75</f>
         <v>1.8</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A69" s="5">
         <v>43739</v>
       </c>
-      <c r="B69" s="4">
-        <v>0</v>
-      </c>
-      <c r="C69" s="8">
+      <c r="B69" s="8">
         <f>所用指标!AD74</f>
         <v>25.318523358379586</v>
       </c>
-      <c r="D69" s="8">
+      <c r="C69" s="8">
         <f>所用指标!AD71</f>
         <v>8.8737904056001682</v>
       </c>
-      <c r="E69" s="9">
+      <c r="D69" s="9">
         <f>所用指标!V76</f>
         <v>-1.2095065092340263</v>
       </c>
-      <c r="F69" s="9">
+      <c r="E69" s="9">
         <f>所用指标!W76</f>
         <v>1.1147018310159185</v>
       </c>
-      <c r="G69" s="8">
+      <c r="F69" s="8">
         <f>所用指标!X75</f>
         <v>19.7</v>
       </c>
-      <c r="H69" s="8">
+      <c r="G69" s="8">
         <f>所用指标!X73</f>
         <v>7.8</v>
       </c>
-      <c r="I69" s="4">
+      <c r="H69" s="4">
         <f>综合!E76</f>
         <v>1.8</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A70" s="5">
         <v>43770</v>
       </c>
-      <c r="B70" s="4">
-        <v>1</v>
-      </c>
-      <c r="C70" s="8">
+      <c r="B70" s="8">
         <f>所用指标!AD75</f>
         <v>7.328467153284679</v>
       </c>
-      <c r="D70" s="8">
+      <c r="C70" s="8">
         <f>所用指标!AD72</f>
         <v>18.66868381240543</v>
       </c>
-      <c r="E70" s="9">
+      <c r="D70" s="9">
         <f>所用指标!V77</f>
         <v>3.7151919654486276</v>
       </c>
-      <c r="F70" s="9">
+      <c r="E70" s="9">
         <f>所用指标!W77</f>
         <v>1.3039023519366033</v>
       </c>
-      <c r="G70" s="8">
+      <c r="F70" s="8">
         <f>所用指标!X76</f>
         <v>20.100000000000001</v>
       </c>
-      <c r="H70" s="8">
+      <c r="G70" s="8">
         <f>所用指标!X74</f>
         <v>23.1</v>
       </c>
-      <c r="I70" s="4">
+      <c r="H70" s="4">
         <f>综合!E77</f>
         <v>1.8</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A71" s="5">
         <v>43800</v>
       </c>
-      <c r="B71" s="4">
-        <v>0</v>
-      </c>
-      <c r="C71" s="8">
+      <c r="B71" s="8">
         <f>所用指标!AD76</f>
         <v>-8.1493859785481177</v>
       </c>
-      <c r="D71" s="8">
+      <c r="C71" s="8">
         <f>所用指标!AD73</f>
         <v>21.948304436512011</v>
       </c>
-      <c r="E71" s="9">
+      <c r="D71" s="9">
         <f>所用指标!V78</f>
         <v>0.23534145376953308</v>
       </c>
-      <c r="F71" s="9">
+      <c r="E71" s="9">
         <f>所用指标!W78</f>
         <v>9.3099633130089288E-3</v>
       </c>
-      <c r="G71" s="8">
+      <c r="F71" s="8">
         <f>所用指标!X77</f>
         <v>3.8</v>
       </c>
-      <c r="H71" s="8">
+      <c r="G71" s="8">
         <f>所用指标!X75</f>
         <v>19.7</v>
       </c>
-      <c r="I71" s="4">
+      <c r="H71" s="4">
         <f>综合!E78</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A72" s="5">
         <v>43831</v>
       </c>
-      <c r="B72" s="4">
-        <v>0</v>
-      </c>
-      <c r="C72" s="8">
+      <c r="B72" s="8">
         <f>所用指标!AD77</f>
         <v>2.2706438191947287</v>
       </c>
-      <c r="D72" s="8">
+      <c r="C72" s="8">
         <f>所用指标!AD74</f>
         <v>25.318523358379586</v>
       </c>
-      <c r="E72" s="9">
+      <c r="D72" s="9">
         <f>所用指标!V79</f>
         <v>2.7840336945183175</v>
       </c>
-      <c r="F72" s="9">
+      <c r="E72" s="9">
         <f>所用指标!W79</f>
         <v>0.80076359635989913</v>
       </c>
-      <c r="G72" s="8">
+      <c r="F72" s="8">
         <f>所用指标!X78</f>
         <v>-5.6</v>
       </c>
-      <c r="H72" s="8">
+      <c r="G72" s="8">
         <f>所用指标!X76</f>
         <v>20.100000000000001</v>
       </c>
-      <c r="I72" s="4">
+      <c r="H72" s="4">
         <f>综合!E79</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A73" s="5">
         <v>43862</v>
       </c>
-      <c r="B73" s="4">
-        <v>0</v>
-      </c>
-      <c r="C73" s="8">
+      <c r="B73" s="8">
         <f>所用指标!AD78</f>
         <v>5.6540026201475468</v>
       </c>
-      <c r="D73" s="8">
+      <c r="C73" s="8">
         <f>所用指标!AD75</f>
         <v>7.328467153284679</v>
       </c>
-      <c r="E73" s="9">
+      <c r="D73" s="9">
         <f>所用指标!V80</f>
         <v>-2.6720765340281227</v>
       </c>
-      <c r="F73" s="9">
+      <c r="E73" s="9">
         <f>所用指标!W80</f>
         <v>0.86640455244992864</v>
       </c>
-      <c r="G73" s="8">
+      <c r="F73" s="8">
         <f>所用指标!X79</f>
         <v>8.5</v>
       </c>
-      <c r="H73" s="8">
+      <c r="G73" s="8">
         <f>所用指标!X77</f>
         <v>3.8</v>
       </c>
-      <c r="I73" s="4">
+      <c r="H73" s="4">
         <f>综合!E80</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A74" s="5">
         <v>43891</v>
       </c>
-      <c r="B74" s="4">
-        <v>0</v>
-      </c>
-      <c r="C74" s="8">
+      <c r="B74" s="8">
         <f>所用指标!AD79</f>
         <v>-0.37525288781572463</v>
       </c>
-      <c r="D74" s="8">
+      <c r="C74" s="8">
         <f>所用指标!AD76</f>
         <v>-8.1493859785481177</v>
       </c>
-      <c r="E74" s="9">
+      <c r="D74" s="9">
         <f>所用指标!V81</f>
         <v>-7.4827627568257338</v>
       </c>
-      <c r="F74" s="9">
+      <c r="E74" s="9">
         <f>所用指标!W81</f>
         <v>-0.20614028563904485</v>
       </c>
-      <c r="G74" s="8">
+      <c r="F74" s="8">
         <f>所用指标!X80</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="H74" s="8">
+      <c r="G74" s="8">
         <f>所用指标!X78</f>
         <v>-5.6</v>
       </c>
-      <c r="I74" s="4">
+      <c r="H74" s="4">
         <f>综合!E81</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A75" s="5">
         <v>43922</v>
       </c>
-      <c r="B75" s="4">
-        <v>0</v>
-      </c>
-      <c r="C75" s="8">
+      <c r="B75" s="8">
         <f>所用指标!AD80</f>
         <v>-4.8196914611378645</v>
       </c>
-      <c r="D75" s="8">
+      <c r="C75" s="8">
         <f>所用指标!AD77</f>
         <v>2.2706438191947287</v>
       </c>
-      <c r="E75" s="9">
+      <c r="D75" s="9">
         <f>所用指标!V82</f>
         <v>-4.7334247300369059</v>
       </c>
-      <c r="F75" s="9">
+      <c r="E75" s="9">
         <f>所用指标!W82</f>
         <v>-2.4770835251259116</v>
       </c>
-      <c r="G75" s="8">
+      <c r="F75" s="8">
         <f>所用指标!X81</f>
         <v>-6.9</v>
       </c>
-      <c r="H75" s="8">
+      <c r="G75" s="8">
         <f>所用指标!X79</f>
         <v>8.5</v>
       </c>
-      <c r="I75" s="4">
+      <c r="H75" s="4">
         <f>综合!E82</f>
         <v>-0.2</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A76" s="5">
         <v>43952</v>
       </c>
-      <c r="B76" s="4">
-        <v>0</v>
-      </c>
-      <c r="C76" s="8">
+      <c r="B76" s="8">
         <f>所用指标!AD81</f>
         <v>-9.8580498632116829</v>
       </c>
-      <c r="D76" s="8">
+      <c r="C76" s="8">
         <f>所用指标!AD78</f>
         <v>5.6540026201475468</v>
       </c>
-      <c r="E76" s="9">
+      <c r="D76" s="9">
         <f>所用指标!V83</f>
         <v>1.9331943439438115</v>
       </c>
-      <c r="F76" s="9">
+      <c r="E76" s="9">
         <f>所用指标!W83</f>
         <v>-0.45698236907580903</v>
       </c>
-      <c r="G76" s="8">
+      <c r="F76" s="8">
         <f>所用指标!X82</f>
         <v>-7.6</v>
       </c>
-      <c r="H76" s="8">
+      <c r="G76" s="8">
         <f>所用指标!X80</f>
         <v>9.3000000000000007</v>
       </c>
-      <c r="I76" s="4">
+      <c r="H76" s="4">
         <f>综合!E83</f>
         <v>-0.8</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A77" s="5">
         <v>43983</v>
       </c>
-      <c r="B77" s="4">
-        <v>0</v>
-      </c>
-      <c r="C77" s="8">
+      <c r="B77" s="8">
         <f>所用指标!AD82</f>
         <v>-2.4176554125246108</v>
       </c>
-      <c r="D77" s="8">
+      <c r="C77" s="8">
         <f>所用指标!AD79</f>
         <v>-0.37525288781572463</v>
       </c>
-      <c r="E77" s="9">
+      <c r="D77" s="9">
         <f>所用指标!V84</f>
         <v>7.6439910784571019</v>
       </c>
-      <c r="F77" s="9">
+      <c r="E77" s="9">
         <f>所用指标!W84</f>
         <v>1.3973701921748072</v>
       </c>
-      <c r="G77" s="8">
+      <c r="F77" s="8">
         <f>所用指标!X83</f>
         <v>-8.1</v>
       </c>
-      <c r="H77" s="8">
+      <c r="G77" s="8">
         <f>所用指标!X81</f>
         <v>-6.9</v>
       </c>
-      <c r="I77" s="4">
+      <c r="H77" s="4">
         <f>综合!E84</f>
         <v>0.4</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A78" s="5">
         <v>44013</v>
       </c>
-      <c r="B78" s="4">
-        <v>0</v>
-      </c>
-      <c r="C78" s="8">
+      <c r="B78" s="8">
         <f>所用指标!AD83</f>
         <v>14.598908514758492</v>
       </c>
-      <c r="D78" s="8">
+      <c r="C78" s="8">
         <f>所用指标!AD80</f>
         <v>-4.8196914611378645</v>
       </c>
-      <c r="E78" s="9">
+      <c r="D78" s="9">
         <f>所用指标!V85</f>
         <v>11.805245053326896</v>
       </c>
-      <c r="F78" s="9">
+      <c r="E78" s="9">
         <f>所用指标!W85</f>
         <v>1.1691126890504888</v>
       </c>
-      <c r="G78" s="8">
+      <c r="F78" s="8">
         <f>所用指标!X84</f>
         <v>3.6</v>
       </c>
-      <c r="H78" s="8">
+      <c r="G78" s="8">
         <f>所用指标!X82</f>
         <v>-7.6</v>
       </c>
-      <c r="I78" s="4">
+      <c r="H78" s="4">
         <f>综合!E85</f>
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.4">
       <c r="A79" s="5">
         <v>44044</v>
       </c>
-      <c r="B79" s="4">
-        <v>0</v>
+      <c r="B79" s="8">
+        <v>7.0258000000000003</v>
       </c>
       <c r="C79" s="8">
-        <v>7.0258000000000003</v>
-      </c>
-      <c r="D79" s="8">
         <f>所用指标!AD81</f>
         <v>-9.8580498632116829</v>
       </c>
-      <c r="E79" s="9">
+      <c r="D79" s="9">
         <f>所用指标!V86</f>
         <v>7.5510599460029137</v>
       </c>
-      <c r="F79" s="9">
+      <c r="E79" s="9">
         <f>所用指标!W86</f>
         <v>2.8773663502008828</v>
       </c>
-      <c r="G79" s="8">
+      <c r="F79" s="8">
         <f>所用指标!X85</f>
         <v>10.3</v>
       </c>
-      <c r="H79" s="8">
+      <c r="G79" s="8">
         <f>所用指标!X83</f>
         <v>-8.1</v>
       </c>
-      <c r="I79" s="4">
+      <c r="H79" s="4">
         <f>综合!E86</f>
         <v>0</v>
       </c>

</xml_diff>